<commit_message>
metadata adjusted and files git status
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aminaly/Box Sync/SDG15.4.1_Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C5F136-2245-904B-82A9-FD3232E1A2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D439246-B7F7-5648-82F6-3ECE1831E503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{DFAF779D-087A-A343-B3FD-AE82D10605A6}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>CountryRange_Highland_KBAPA_GMBA_Area</t>
   </si>
   <si>
-    <t>File</t>
-  </si>
-  <si>
     <t>clean_data_for_visuals_range_MONTHYEAR.csv</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>Updated Annually?</t>
-  </si>
-  <si>
     <t>Variable Name in Code</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>File with KBA classification information</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>tabmf</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>File with ISO country codes and their country of origin</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>isos</t>
   </si>
   <si>
@@ -186,9 +174,6 @@
     <t>Filtered WDPA data as provided directly by WCMC</t>
   </si>
   <si>
-    <t>Yes*</t>
-  </si>
-  <si>
     <t>pas</t>
   </si>
   <si>
@@ -234,9 +219,6 @@
     <t>Intersection_GMBA</t>
   </si>
   <si>
-    <t>Shapefile with country outlines. Used only for visualisation associated with debugging. Country assignments are still based on the ISO code in KBA, GMBA, and PA files</t>
-  </si>
-  <si>
     <t>/results/results_mt/</t>
   </si>
   <si>
@@ -529,6 +511,24 @@
   </si>
   <si>
     <t>Area-Based KBA Coverage by PAs for each GMBA Mountain System (Basic, conservative mountain definition) AND Country. KBAs are cropped by GMBA Mountain</t>
+  </si>
+  <si>
+    <t>By request</t>
+  </si>
+  <si>
+    <t>Update Period</t>
+  </si>
+  <si>
+    <t>Semi-annual</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> File Name (/results/File_Name.csv)</t>
+  </si>
+  <si>
+    <t>OPTIONAL Shapefile with country outlines. Used only for visualisation associated with debugging. Can be any world shapefile with ISO codes. Country assignments are still based on the ISO code in KBA, GMBA, and PA files</t>
   </si>
 </sst>
 </file>
@@ -947,7 +947,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,223 +963,223 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -1227,7 +1227,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1240,72 +1240,72 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="5" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1349,10 +1349,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1360,10 +1360,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1371,10 +1371,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1382,10 +1382,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1393,10 +1393,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1404,10 +1404,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1415,10 +1415,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1426,10 +1426,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1437,76 +1437,76 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" t="s">
         <v>151</v>
-      </c>
-      <c r="B11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" t="s">
         <v>154</v>
-      </c>
-      <c r="B14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" t="s">
         <v>155</v>
-      </c>
-      <c r="B15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>156</v>
-      </c>
-      <c r="B16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1534,108 +1534,108 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="M1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" s="13" t="s">
+      <c r="P1" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="M2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q2" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1677,126 +1677,126 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="M2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1859,43 +1859,43 @@
   <sheetData>
     <row r="1" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="H1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>126</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>132</v>
       </c>
       <c r="N1" s="14" t="s">
         <v>0</v>
@@ -1904,46 +1904,46 @@
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="H2" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="K2" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="M2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="O2" s="9"/>
     </row>

</xml_diff>